<commit_message>
commit changes into excel setup and also formatting of dates
</commit_message>
<xml_diff>
--- a/testData/UserData.xlsx
+++ b/testData/UserData.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21000" windowHeight="11160"/>
+    <workbookView windowWidth="28800" windowHeight="12210" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="UserCredentials" sheetId="1" r:id="rId1"/>
+    <sheet name="SearchHotel" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Username</t>
   </si>
@@ -26,20 +27,74 @@
   </si>
   <si>
     <t>password</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Hotels</t>
+  </si>
+  <si>
+    <t>RoomTypes</t>
+  </si>
+  <si>
+    <t>NumberOfRooms</t>
+  </si>
+  <si>
+    <t>CheckInDate</t>
+  </si>
+  <si>
+    <t>CheckOutDate</t>
+  </si>
+  <si>
+    <t>AdultPerRoom</t>
+  </si>
+  <si>
+    <t>ChildrenPerRoom</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Hotel Sunshine</t>
+  </si>
+  <si>
+    <t>Double</t>
+  </si>
+  <si>
+    <t>4 - Four</t>
+  </si>
+  <si>
+    <t>22/12/2023</t>
+  </si>
+  <si>
+    <t>2 - Two</t>
+  </si>
+  <si>
+    <t>1 - One</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="m/d/yyyy;@"/>
   </numFmts>
-  <fonts count="20">
-    <font>
+  <fonts count="21">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -200,13 +255,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -521,140 +576,149 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -996,7 +1060,7 @@
   <sheetPr/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -1007,10 +1071,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1026,4 +1090,83 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="9.875" customWidth="1"/>
+    <col min="2" max="2" width="15.125" customWidth="1"/>
+    <col min="3" max="3" width="13.25" customWidth="1"/>
+    <col min="4" max="4" width="17.5" customWidth="1"/>
+    <col min="5" max="5" width="13.375" customWidth="1"/>
+    <col min="6" max="6" width="14.75" customWidth="1"/>
+    <col min="7" max="7" width="14.875" customWidth="1"/>
+    <col min="8" max="8" width="18.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="3">
+        <v>45352</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
commit more method to finish end to end testing
</commit_message>
<xml_diff>
--- a/testData/UserData.xlsx
+++ b/testData/UserData.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12210" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="12210" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="UserCredentials" sheetId="1" r:id="rId1"/>
     <sheet name="SearchHotel" sheetId="3" r:id="rId2"/>
+    <sheet name="BookHotel" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Username</t>
   </si>
@@ -72,6 +73,48 @@
   </si>
   <si>
     <t>1 - One</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>BillingAddress</t>
+  </si>
+  <si>
+    <t>CreditCardNumber</t>
+  </si>
+  <si>
+    <t>CreditCardType</t>
+  </si>
+  <si>
+    <t>ExpiryMonth</t>
+  </si>
+  <si>
+    <t>ExpiryYear</t>
+  </si>
+  <si>
+    <t>CVVNumber</t>
+  </si>
+  <si>
+    <t>Peaky</t>
+  </si>
+  <si>
+    <t>Blinders</t>
+  </si>
+  <si>
+    <t>23 Avenue, Noordwyk, Midrand, 1682</t>
+  </si>
+  <si>
+    <t>5344740012554980</t>
+  </si>
+  <si>
+    <t>VISA</t>
+  </si>
+  <si>
+    <t>November</t>
   </si>
 </sst>
 </file>
@@ -706,7 +749,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -714,11 +757,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" quotePrefix="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1071,10 +1123,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1097,8 +1149,8 @@
   <sheetPr/>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="7"/>
@@ -1152,10 +1204,10 @@
       <c r="D2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="5">
         <v>45352</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -1163,6 +1215,85 @@
       </c>
       <c r="H2" s="2" t="s">
         <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="11.625" customWidth="1"/>
+    <col min="2" max="2" width="12.75" customWidth="1"/>
+    <col min="3" max="3" width="33.5" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="16.25" customWidth="1"/>
+    <col min="6" max="6" width="16.5" customWidth="1"/>
+    <col min="7" max="7" width="11.25" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="30" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2">
+        <v>2029</v>
+      </c>
+      <c r="H2">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>